<commit_message>
Update VTI TI4 stems
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VTA-splitstem.xlsx
+++ b/inc/flattened/createYaml/VTA-splitstem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FAE629-8715-AF4F-8D30-BF9157F2071B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9494DBAA-357D-984F-8898-1BFBFB68F28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26840" yWindow="5060" windowWidth="26840" windowHeight="14860" activeTab="1" xr2:uid="{9DF8881B-D06D-0846-BEE5-CCB34DBF0AD0}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{9DF8881B-D06D-0846-BEE5-CCB34DBF0AD0}"/>
   </bookViews>
   <sheets>
     <sheet name="VTA_IND" sheetId="1" r:id="rId1"/>
@@ -6107,12 +6107,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -6127,11 +6133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6448,8 +6455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344DB255-9D86-DF46-82C2-AB3642BC0317}">
   <dimension ref="A1:J1831"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J145" sqref="J145"/>
+    <sheetView tabSelected="1" topLeftCell="A1127" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I1779" sqref="I1779"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40220,7 +40227,7 @@
       <c r="H1160" t="s">
         <v>10</v>
       </c>
-      <c r="I1160" s="2" t="s">
+      <c r="I1160" s="4" t="s">
         <v>1672</v>
       </c>
     </row>
@@ -40249,7 +40256,7 @@
       <c r="H1161" t="s">
         <v>9</v>
       </c>
-      <c r="I1161" s="2" t="s">
+      <c r="I1161" s="4" t="s">
         <v>1673</v>
       </c>
     </row>
@@ -59701,7 +59708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844F8B8D-B51F-F84E-96B1-1FA656EE28D3}">
   <dimension ref="A1:J319"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A321" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update yaml generator and excel for VTAs
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VTA-splitstem.xlsx
+++ b/inc/flattened/createYaml/VTA-splitstem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767041EF-F551-EA48-8D88-6345F0E62F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC524DC-B771-3647-AB0D-00CCB7BE62F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{9DF8881B-D06D-0846-BEE5-CCB34DBF0AD0}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{9DF8881B-D06D-0846-BEE5-CCB34DBF0AD0}"/>
   </bookViews>
   <sheets>
     <sheet name="VTA_IND" sheetId="1" r:id="rId1"/>
@@ -6413,7 +6413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344DB255-9D86-DF46-82C2-AB3642BC0317}">
   <dimension ref="A1:J1831"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1260" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="D1267" zoomScale="150" workbookViewId="0">
       <selection activeCell="I1153" sqref="I1153"/>
     </sheetView>
   </sheetViews>
@@ -59666,7 +59666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844F8B8D-B51F-F84E-96B1-1FA656EE28D3}">
   <dimension ref="A1:J319"/>
   <sheetViews>
-    <sheetView topLeftCell="A321" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Small updates to spreadsheets
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VTA-splitstem.xlsx
+++ b/inc/flattened/createYaml/VTA-splitstem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E726BE63-8A13-D140-BB68-751C9B312B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35C4114-0BE0-804A-96EB-40BA0F35984C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{9DF8881B-D06D-0846-BEE5-CCB34DBF0AD0}"/>
   </bookViews>
@@ -6412,8 +6412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344DB255-9D86-DF46-82C2-AB3642BC0317}">
   <dimension ref="A1:J1831"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1076" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D734" sqref="D734:D1099"/>
+    <sheetView tabSelected="1" topLeftCell="A999" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I1024" sqref="I1024"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>